<commit_message>
call me adderall the way i'm adding all this shit
</commit_message>
<xml_diff>
--- a/cad/plano de processos.xlsx
+++ b/cad/plano de processos.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04953341a4623d5c/aviãozinho/monociclo/mono/cad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{97C0245A-1B82-4EFD-B808-07D57EC8638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F5D9A5A-0D4C-49C9-96A0-761C63581724}"/>
+  <xr:revisionPtr revIDLastSave="321" documentId="8_{97C0245A-1B82-4EFD-B808-07D57EC8638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA0FD77-3FCA-4A47-BF82-26AC0F7045B3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EA45038B-2C59-4707-B715-C80FE21208D7}"/>
   </bookViews>
   <sheets>
     <sheet name="peça acopladora" sheetId="4" r:id="rId1"/>
-    <sheet name="bucha" sheetId="15" r:id="rId2"/>
+    <sheet name="eixo" sheetId="15" r:id="rId2"/>
     <sheet name="c-hub" sheetId="14" r:id="rId3"/>
     <sheet name="corpo" sheetId="16" r:id="rId4"/>
     <sheet name="ex_Sub-Operações" sheetId="10" r:id="rId5"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="173">
   <si>
     <t>Operação</t>
   </si>
@@ -832,9 +832,6 @@
     <t>Fresamento do furo 12mm</t>
   </si>
   <si>
-    <t>Torno convencional</t>
-  </si>
-  <si>
     <t>placa de três castanhas</t>
   </si>
   <si>
@@ -925,9 +922,6 @@
     <t>Matéria-prima: alumínio 5052 - 1.1/2" x 30mm</t>
   </si>
   <si>
-    <t>Prismática convencional</t>
-  </si>
-  <si>
     <t>Rosqueamento</t>
   </si>
   <si>
@@ -974,10 +968,103 @@
     <t>Matéria-prima: alumínio 5052 - 2" x 25mm</t>
   </si>
   <si>
-    <t>Peça: bucha</t>
-  </si>
-  <si>
-    <t>Matéria-prima: alumínio 5052 - 1" x 40mm</t>
+    <t>Torno GL</t>
+  </si>
+  <si>
+    <t>ap = .667mm
+vc = 165m/min
+f = .197mm
+n = 6000rpm</t>
+  </si>
+  <si>
+    <t>deixar com 15mm para fora</t>
+  </si>
+  <si>
+    <t>Faceamento (desbaste e acabamento)</t>
+  </si>
+  <si>
+    <t>ap = .952mm
+vc = 165m/min
+f = .194mm
+n = 1970rpm</t>
+  </si>
+  <si>
+    <t>ap = .839mm
+vc = 165m/min
+f = .194mm
+n = 2110rpm</t>
+  </si>
+  <si>
+    <t>Vekker</t>
+  </si>
+  <si>
+    <t>A2002.5X6.3</t>
+  </si>
+  <si>
+    <t>ap = ?
+vc = 33m/min
+f = .11mm</t>
+  </si>
+  <si>
+    <t>A1003.5</t>
+  </si>
+  <si>
+    <t>ap = ?
+vc = 33m/min
+f = .144mm</t>
+  </si>
+  <si>
+    <t>Inserto VCGT160408-PM2-WK1</t>
+  </si>
+  <si>
+    <t>Peça: eixo</t>
+  </si>
+  <si>
+    <t>Matéria-prima: aço 1045 - 2" x 120mm</t>
+  </si>
+  <si>
+    <t>Furação 5xM3</t>
+  </si>
+  <si>
+    <t>Sangramento</t>
+  </si>
+  <si>
+    <t>Furação 5x rebaixo</t>
+  </si>
+  <si>
+    <t>A1002.5</t>
+  </si>
+  <si>
+    <t>A1006.5</t>
+  </si>
+  <si>
+    <t>ap = .667mm
+vc = 172m/min
+f = .197mm
+n = 4000rpm</t>
+  </si>
+  <si>
+    <t>ap = .666mm
+vc = 172m/min
+f = .197mm
+n = 4000rpm</t>
+  </si>
+  <si>
+    <t>ap = .267mm
+vc = 172m/min
+f = .261mm
+n = 4000rpm</t>
+  </si>
+  <si>
+    <t>ap = .666mm
+vc = 179m/min
+f = .101mm
+n = 4000rpm</t>
+  </si>
+  <si>
+    <t>ap = ?
+vc = 33m/min
+f = .21mm</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1162,6 +1249,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1539,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C174505-2944-4897-B3FF-59AEE70B3D2A}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -1572,7 +1665,7 @@
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
@@ -1608,10 +1701,10 @@
         <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1622,10 +1715,10 @@
         <v>88</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1636,10 +1729,10 @@
         <v>102</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1651,7 +1744,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1662,10 +1755,10 @@
         <v>104</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1677,7 +1770,7 @@
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1688,10 +1781,10 @@
         <v>106</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1702,10 +1795,10 @@
         <v>107</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1716,10 +1809,10 @@
         <v>108</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1730,10 +1823,10 @@
         <v>109</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1744,10 +1837,10 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1758,7 +1851,7 @@
         <v>111</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1771,11 +1864,11 @@
         <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="50.4" x14ac:dyDescent="0.2">
@@ -1785,10 +1878,10 @@
         <v>88</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1799,11 +1892,11 @@
         <v>102</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="25.2" x14ac:dyDescent="0.2">
@@ -1823,26 +1916,26 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B4:B19"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A15"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B4:B19"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1851,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E0EFCA-FCFF-424E-9955-4088D441A37C}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -1881,12 +1974,12 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
@@ -1911,11 +2004,143 @@
         <v>58</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="A4:A13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1924,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F046EA98-9569-4131-B880-DABB63529D60}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D4:D14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -1954,12 +2179,12 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
@@ -1984,18 +2209,20 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
@@ -2006,115 +2233,125 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.2" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="25.2" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+        <v>139</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <v>3</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="37.799999999999997" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
+  <mergeCells count="8">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="B4:B10"/>
     <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2153,12 +2390,12 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
@@ -2188,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>

</xml_diff>